<commit_message>
updated excel sheet of 8 nov
</commit_message>
<xml_diff>
--- a/CMS_Issue_List_8-11-2017.xlsx
+++ b/CMS_Issue_List_8-11-2017.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" firstSheet="16" activeTab="22"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" firstSheet="17" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="16-06-2017" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,7 @@
     <sheet name="27-10-2017" sheetId="21" r:id="rId21"/>
     <sheet name="1-11-2017" sheetId="22" r:id="rId22"/>
     <sheet name="8-11-2017" sheetId="23" r:id="rId23"/>
+    <sheet name="22-11-2017" sheetId="24" r:id="rId24"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6">'14-06-2017'!$A$2:$F$24</definedName>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1383" uniqueCount="451">
   <si>
     <t>Module</t>
   </si>
@@ -1434,6 +1435,12 @@
   </si>
   <si>
     <t>should not accept mobile number  a same number as a "9999999999"</t>
+  </si>
+  <si>
+    <t>CMS WEB TESTING REPORT OF NEW FEATURE AS BOOTH LEVEL IN BULCKUPLOAD</t>
+  </si>
+  <si>
+    <t>should not accept spaces in the middle of email field</t>
   </si>
 </sst>
 </file>
@@ -5650,8 +5657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5972,7 +5979,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -6155,6 +6162,85 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" customWidth="1"/>
+    <col min="3" max="3" width="54.28515625" customWidth="1"/>
+    <col min="4" max="4" width="51.28515625" customWidth="1"/>
+    <col min="7" max="7" width="37.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="38"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38" t="s">
+        <v>449</v>
+      </c>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+    </row>
+    <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>144</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="44" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3" t="s">
+        <v>402</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>271</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>450</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>